<commit_message>
finished fixing DE data
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_DE.xlsx
+++ b/in/extraction1/corrections/supp_DE.xlsx
@@ -16015,17 +16015,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -26198,7 +26188,7 @@
   </sheetData>
   <autoFilter ref="A1:P102"/>
   <conditionalFormatting sqref="C2:C89">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26209,8 +26199,8 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29665,7 +29655,7 @@
         <v>38151</v>
       </c>
       <c r="K69" s="16">
-        <v>39844</v>
+        <v>39970</v>
       </c>
       <c r="L69" s="15" t="s">
         <v>256</v>
@@ -30312,7 +30302,7 @@
         <v>4968</v>
       </c>
       <c r="J82" s="16">
-        <v>39729</v>
+        <v>39722</v>
       </c>
       <c r="K82" s="16">
         <v>39970</v>

</xml_diff>

<commit_message>
updated D correction data
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_DE.xlsx
+++ b/in/extraction1/corrections/supp_DE.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10953" uniqueCount="5446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10953" uniqueCount="5447">
   <si>
     <t>Code sexe</t>
   </si>
@@ -16371,6 +16371,9 @@
   </si>
   <si>
     <t>EUR_0000962</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
@@ -21860,7 +21863,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J111" sqref="J111"/>
+      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22918,7 +22921,7 @@
         <v>33829</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>382</v>
+        <v>5446</v>
       </c>
       <c r="M21" s="15" t="s">
         <v>5291</v>
@@ -23418,7 +23421,7 @@
         <v>33790</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>382</v>
+        <v>5446</v>
       </c>
       <c r="M31" s="15" t="s">
         <v>513</v>

</xml_diff>